<commit_message>
argentinian added on database
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">Argentine</t>
+    <t xml:space="preserve">Argentinian</t>
   </si>
   <si>
     <t xml:space="preserve">Spanish</t>
@@ -1495,7 +1495,7 @@
   <dimension ref="A1:S255"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>